<commit_message>
os separators change to nix-like and del unnecessary strings
</commit_message>
<xml_diff>
--- a/resources/example.xlsx
+++ b/resources/example.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Seventh Edition</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>Дополнительно</t>
+  </si>
+  <si>
+    <t>Conflux</t>
+  </si>
+  <si>
+    <t>Впитать Мощь</t>
+  </si>
+  <si>
+    <t>Asha's Favor</t>
   </si>
 </sst>
 </file>
@@ -443,11 +452,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -645,6 +654,28 @@
       </c>
       <c r="D15" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>